<commit_message>
first version of clock-stop model added
</commit_message>
<xml_diff>
--- a/data/capacity_table.xlsx
+++ b/data/capacity_table.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\src\work-time-model-psy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5C293C7-7AB4-41B7-A9C5-B17FE8604856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F914B2-7EFA-49E3-9027-58D62AF73C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA13BA64-248C-48A0-B80E-08D31A577A73}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="capacity" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>service</t>
   </si>
@@ -52,6 +51,18 @@
   </si>
   <si>
     <t>Assessment</t>
+  </si>
+  <si>
+    <t>MBT</t>
+  </si>
+  <si>
+    <t>SCM</t>
+  </si>
+  <si>
+    <t>Liaison</t>
+  </si>
+  <si>
+    <t>Med-RV</t>
   </si>
 </sst>
 </file>
@@ -403,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E91BFA-B15B-4D3D-991D-A2AD2650B1DB}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,16 +450,96 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <v>16</v>
       </c>
-      <c r="D2">
-        <v>220</v>
-      </c>
-      <c r="E2">
-        <v>77</v>
+      <c r="D3">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f>365+250</f>
+        <v>615</v>
+      </c>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <f>365+30+30+250</f>
+        <v>675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>